<commit_message>
Merged  satisfaction values and the mobidity rate and churn rate tables
</commit_message>
<xml_diff>
--- a/data/custom_files/kundenmonitor_churn_merged.xlsx
+++ b/data/custom_files/kundenmonitor_churn_merged.xlsx
@@ -130,7 +130,7 @@
     <t>Kundenmagazin Gesamtzufriedenheit</t>
   </si>
   <si>
-    <t>Year</t>
+    <t>Jahr</t>
   </si>
   <si>
     <t>Churn_Rate_2023</t>
@@ -373,7 +373,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -426,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -440,17 +440,14 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -772,50 +769,50 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="11" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="35" max="35" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="36" max="36" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="38" max="38" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="39" max="39" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="40" max="40" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="41" max="41" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="35" max="35" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="36" max="36" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="38" max="38" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="39" max="39" style="11" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="40" max="40" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="41" max="41" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9122,7 +9119,7 @@
       <c r="E68" s="5">
         <v>3.07285576715462</v>
       </c>
-      <c r="F68" s="8"/>
+      <c r="F68" s="7"/>
       <c r="G68" s="5">
         <v>2.04095438896127</v>
       </c>
@@ -9602,7 +9599,7 @@
       <c r="E72" s="5">
         <v>2.50986245868727</v>
       </c>
-      <c r="F72" s="8"/>
+      <c r="F72" s="7"/>
       <c r="G72" s="5">
         <v>2.1990484260319</v>
       </c>
@@ -9975,7 +9972,7 @@
       <c r="E75" s="5">
         <v>2.42971793193359</v>
       </c>
-      <c r="F75" s="8"/>
+      <c r="F75" s="7"/>
       <c r="G75" s="5">
         <v>2.50483378709952</v>
       </c>
@@ -10465,7 +10462,7 @@
       <c r="E79" s="5">
         <v>2.34673999091219</v>
       </c>
-      <c r="F79" s="8"/>
+      <c r="F79" s="7"/>
       <c r="G79" s="5">
         <v>2.03172070789541</v>
       </c>
@@ -10713,7 +10710,7 @@
       <c r="E81" s="5">
         <v>2.38570484110314</v>
       </c>
-      <c r="F81" s="8"/>
+      <c r="F81" s="7"/>
       <c r="G81" s="5">
         <v>2.15497113760556</v>
       </c>
@@ -11457,7 +11454,7 @@
       <c r="E87" s="5">
         <v>2.40718438506975</v>
       </c>
-      <c r="F87" s="8"/>
+      <c r="F87" s="7"/>
       <c r="G87" s="5">
         <v>1.96658863519428</v>
       </c>
@@ -11955,7 +11952,7 @@
       <c r="E91" s="5">
         <v>2.21205205313545</v>
       </c>
-      <c r="F91" s="8"/>
+      <c r="F91" s="7"/>
       <c r="G91" s="5">
         <v>2.00808650197343</v>
       </c>
@@ -12203,7 +12200,7 @@
       <c r="E93" s="5">
         <v>2.36032001382547</v>
       </c>
-      <c r="F93" s="8"/>
+      <c r="F93" s="7"/>
       <c r="G93" s="5">
         <v>2.06287818755332</v>
       </c>
@@ -12326,7 +12323,7 @@
       <c r="E94" s="5">
         <v>2.24635677815632</v>
       </c>
-      <c r="F94" s="8"/>
+      <c r="F94" s="7"/>
       <c r="G94" s="5">
         <v>1.87724584374701</v>
       </c>
@@ -12816,7 +12813,7 @@
       <c r="E98" s="5">
         <v>2.56787528310196</v>
       </c>
-      <c r="F98" s="8"/>
+      <c r="F98" s="7"/>
       <c r="G98" s="5">
         <v>2.02024470585687</v>
       </c>
@@ -12939,7 +12936,7 @@
       <c r="E99" s="5">
         <v>2.14903414862276</v>
       </c>
-      <c r="F99" s="8"/>
+      <c r="F99" s="7"/>
       <c r="G99" s="5">
         <v>1.70604418648824</v>
       </c>
@@ -13308,7 +13305,7 @@
       <c r="E102" s="5">
         <v>2.11277407372031</v>
       </c>
-      <c r="F102" s="8"/>
+      <c r="F102" s="7"/>
       <c r="G102" s="5">
         <v>2.01346621616587</v>
       </c>
@@ -13431,7 +13428,7 @@
       <c r="E103" s="5">
         <v>2.11055841526038</v>
       </c>
-      <c r="F103" s="8"/>
+      <c r="F103" s="7"/>
       <c r="G103" s="5">
         <v>1.920077116501</v>
       </c>
@@ -13804,7 +13801,7 @@
       <c r="E106" s="5">
         <v>2.32805616085852</v>
       </c>
-      <c r="F106" s="8"/>
+      <c r="F106" s="7"/>
       <c r="G106" s="5">
         <v>2.06126161036316</v>
       </c>
@@ -13927,7 +13924,7 @@
       <c r="E107" s="5">
         <v>2.37732719488878</v>
       </c>
-      <c r="F107" s="8"/>
+      <c r="F107" s="7"/>
       <c r="G107" s="5">
         <v>2.12827434090738</v>
       </c>
@@ -14050,7 +14047,7 @@
       <c r="E108" s="5">
         <v>2.27886941881962</v>
       </c>
-      <c r="F108" s="8"/>
+      <c r="F108" s="7"/>
       <c r="G108" s="5">
         <v>1.89465230432216</v>
       </c>
@@ -15526,7 +15523,7 @@
       <c r="E120" s="5">
         <v>2.0420778154993</v>
       </c>
-      <c r="F120" s="8"/>
+      <c r="F120" s="7"/>
       <c r="G120" s="5">
         <v>1.74947016147058</v>
       </c>
@@ -15649,7 +15646,7 @@
       <c r="E121" s="5">
         <v>2.09353300069324</v>
       </c>
-      <c r="F121" s="8"/>
+      <c r="F121" s="7"/>
       <c r="G121" s="5">
         <v>2.02443792030353</v>
       </c>
@@ -15895,7 +15892,7 @@
       <c r="E123" s="5">
         <v>1.95035425912416</v>
       </c>
-      <c r="F123" s="8"/>
+      <c r="F123" s="7"/>
       <c r="G123" s="5">
         <v>1.80458103300663</v>
       </c>
@@ -16018,7 +16015,7 @@
       <c r="E124" s="5">
         <v>1.79732863508297</v>
       </c>
-      <c r="F124" s="8"/>
+      <c r="F124" s="7"/>
       <c r="G124" s="5">
         <v>1.84151006308011</v>
       </c>
@@ -16141,7 +16138,7 @@
       <c r="E125" s="5">
         <v>1.45357975512744</v>
       </c>
-      <c r="F125" s="8"/>
+      <c r="F125" s="7"/>
       <c r="G125" s="5">
         <v>1.42660887898743</v>
       </c>

</xml_diff>